<commit_message>
readjusted algorithm based on result testing
</commit_message>
<xml_diff>
--- a/tool/sustainalize/Longlist V2.xlsx
+++ b/tool/sustainalize/Longlist V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hornr\source\repos\openmasses\tool\sustainalize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8197B597-8BEB-4029-A507-810CB24CA01B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{599A2454-975A-4541-BC9C-328996121CD9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="422">
   <si>
     <t>Topic</t>
   </si>
@@ -1264,6 +1264,30 @@
   </si>
   <si>
     <t>Show people that doing good and being successful are not mutually exclusive</t>
+  </si>
+  <si>
+    <t>Partnerships</t>
+  </si>
+  <si>
+    <t>thing1</t>
+  </si>
+  <si>
+    <t>thing2</t>
+  </si>
+  <si>
+    <t>thing3</t>
+  </si>
+  <si>
+    <t>thing4</t>
+  </si>
+  <si>
+    <t>thing5</t>
+  </si>
+  <si>
+    <t>thing6</t>
+  </si>
+  <si>
+    <t>new  fancy knowledge creation</t>
   </si>
 </sst>
 </file>
@@ -1774,11 +1798,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K945"/>
+  <dimension ref="A1:K944"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1853,7 +1877,7 @@
         <v>51</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>48</v>
+        <v>421</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
@@ -2072,7 +2096,9 @@
       <c r="A14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="10"/>
+      <c r="B14" s="24" t="s">
+        <v>414</v>
+      </c>
       <c r="C14" s="10"/>
       <c r="D14" s="25"/>
       <c r="E14" s="28"/>
@@ -2398,7 +2424,7 @@
       <c r="B29" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="C29" s="31"/>
+      <c r="C29" s="43"/>
       <c r="D29" s="32"/>
       <c r="E29" s="40"/>
       <c r="F29" s="34"/>
@@ -2415,7 +2441,9 @@
       <c r="B30" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="C30" s="31"/>
+      <c r="C30" s="43" t="s">
+        <v>415</v>
+      </c>
       <c r="D30" s="32"/>
       <c r="E30" s="40"/>
       <c r="F30" s="34"/>
@@ -2434,7 +2462,9 @@
       <c r="B31" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="C31" s="31"/>
+      <c r="C31" s="43" t="s">
+        <v>416</v>
+      </c>
       <c r="D31" s="32"/>
       <c r="E31" s="33"/>
       <c r="F31" s="34"/>
@@ -2453,7 +2483,9 @@
       <c r="B32" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="C32" s="31"/>
+      <c r="C32" s="43" t="s">
+        <v>417</v>
+      </c>
       <c r="D32" s="32"/>
       <c r="E32" s="40"/>
       <c r="F32" s="34"/>
@@ -2472,7 +2504,9 @@
       <c r="B33" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="C33" s="31"/>
+      <c r="C33" s="43" t="s">
+        <v>418</v>
+      </c>
       <c r="D33" s="32"/>
       <c r="E33" s="40"/>
       <c r="F33" s="34"/>
@@ -2491,7 +2525,9 @@
       <c r="B34" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="C34" s="31"/>
+      <c r="C34" s="43" t="s">
+        <v>419</v>
+      </c>
       <c r="D34" s="32"/>
       <c r="E34" s="33"/>
       <c r="F34" s="34"/>
@@ -2510,7 +2546,9 @@
       <c r="B35" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="C35" s="31"/>
+      <c r="C35" s="43" t="s">
+        <v>420</v>
+      </c>
       <c r="D35" s="32"/>
       <c r="E35" s="33"/>
       <c r="F35" s="34"/>
@@ -2884,12 +2922,20 @@
       <c r="K52" s="9"/>
     </row>
     <row r="53" spans="1:11" ht="12.75">
-      <c r="A53" s="54"/>
-      <c r="B53" s="54"/>
-      <c r="C53" s="52"/>
+      <c r="A53" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="B53" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="C53" s="54" t="s">
+        <v>273</v>
+      </c>
       <c r="D53" s="44"/>
       <c r="E53" s="45"/>
-      <c r="G53" s="8"/>
+      <c r="G53" s="8" t="s">
+        <v>275</v>
+      </c>
       <c r="H53" s="8"/>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
@@ -2899,18 +2945,17 @@
       <c r="A54" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="53" t="s">
+      <c r="B54" s="52" t="s">
         <v>271</v>
       </c>
       <c r="C54" s="54" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="D54" s="44"/>
       <c r="E54" s="45"/>
       <c r="G54" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="H54" s="8"/>
+        <v>279</v>
+      </c>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
@@ -2920,16 +2965,13 @@
         <v>31</v>
       </c>
       <c r="B55" s="52" t="s">
-        <v>271</v>
-      </c>
-      <c r="C55" s="54" t="s">
-        <v>277</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="C55" s="52"/>
       <c r="D55" s="44"/>
       <c r="E55" s="45"/>
-      <c r="G55" s="8" t="s">
-        <v>279</v>
-      </c>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
@@ -2941,9 +2983,11 @@
       <c r="B56" s="52" t="s">
         <v>281</v>
       </c>
-      <c r="C56" s="52"/>
+      <c r="C56" s="52" t="s">
+        <v>32</v>
+      </c>
       <c r="D56" s="44"/>
-      <c r="E56" s="45"/>
+      <c r="E56" s="47"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
       <c r="I56" s="9"/>
@@ -2960,9 +3004,11 @@
       <c r="C57" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="44"/>
+      <c r="D57" s="56"/>
       <c r="E57" s="47"/>
-      <c r="G57" s="9"/>
+      <c r="G57" s="8" t="s">
+        <v>287</v>
+      </c>
       <c r="H57" s="9"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
@@ -2978,10 +3024,12 @@
       <c r="C58" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="D58" s="56"/>
-      <c r="E58" s="47"/>
+      <c r="D58" s="56" t="s">
+        <v>291</v>
+      </c>
+      <c r="E58" s="45"/>
       <c r="G58" s="8" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
@@ -2995,15 +3043,13 @@
       <c r="B59" s="52" t="s">
         <v>281</v>
       </c>
-      <c r="C59" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="D59" s="56" t="s">
-        <v>291</v>
-      </c>
+      <c r="C59" s="54" t="s">
+        <v>296</v>
+      </c>
+      <c r="D59" s="44"/>
       <c r="E59" s="45"/>
-      <c r="G59" s="8" t="s">
-        <v>293</v>
+      <c r="G59" s="61" t="s">
+        <v>296</v>
       </c>
       <c r="H59" s="9"/>
       <c r="I59" s="9"/>
@@ -3018,12 +3064,12 @@
         <v>281</v>
       </c>
       <c r="C60" s="54" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="D60" s="44"/>
-      <c r="E60" s="45"/>
-      <c r="G60" s="61" t="s">
-        <v>296</v>
+      <c r="E60" s="47"/>
+      <c r="G60" s="8" t="s">
+        <v>302</v>
       </c>
       <c r="H60" s="9"/>
       <c r="I60" s="9"/>
@@ -3037,16 +3083,19 @@
       <c r="B61" s="52" t="s">
         <v>281</v>
       </c>
-      <c r="C61" s="54" t="s">
-        <v>302</v>
-      </c>
-      <c r="D61" s="44"/>
+      <c r="C61" s="52" t="s">
+        <v>305</v>
+      </c>
       <c r="E61" s="47"/>
       <c r="G61" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
+        <v>307</v>
+      </c>
+      <c r="H61" s="41" t="s">
+        <v>305</v>
+      </c>
+      <c r="I61" s="56" t="s">
+        <v>308</v>
+      </c>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
     </row>
@@ -3057,19 +3106,16 @@
       <c r="B62" s="52" t="s">
         <v>281</v>
       </c>
-      <c r="C62" s="52" t="s">
-        <v>305</v>
-      </c>
-      <c r="E62" s="47"/>
-      <c r="G62" s="8" t="s">
-        <v>307</v>
-      </c>
-      <c r="H62" s="41" t="s">
-        <v>305</v>
-      </c>
-      <c r="I62" s="56" t="s">
-        <v>308</v>
-      </c>
+      <c r="C62" s="54" t="s">
+        <v>310</v>
+      </c>
+      <c r="D62" s="44"/>
+      <c r="E62" s="45"/>
+      <c r="G62" s="60" t="s">
+        <v>312</v>
+      </c>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
     </row>
@@ -3083,10 +3129,11 @@
       <c r="C63" s="54" t="s">
         <v>310</v>
       </c>
-      <c r="D63" s="44"/>
-      <c r="E63" s="45"/>
-      <c r="G63" s="60" t="s">
-        <v>312</v>
+      <c r="D63" s="62" t="s">
+        <v>313</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>313</v>
       </c>
       <c r="H63" s="9"/>
       <c r="I63" s="9"/>
@@ -3101,13 +3148,12 @@
         <v>281</v>
       </c>
       <c r="C64" s="54" t="s">
-        <v>310</v>
-      </c>
-      <c r="D64" s="62" t="s">
-        <v>313</v>
-      </c>
-      <c r="G64" s="8" t="s">
-        <v>313</v>
+        <v>319</v>
+      </c>
+      <c r="D64" s="44"/>
+      <c r="E64" s="45"/>
+      <c r="G64" s="61" t="s">
+        <v>321</v>
       </c>
       <c r="H64" s="9"/>
       <c r="I64" s="9"/>
@@ -3121,13 +3167,12 @@
       <c r="B65" s="52" t="s">
         <v>281</v>
       </c>
-      <c r="C65" s="54" t="s">
-        <v>319</v>
-      </c>
-      <c r="D65" s="44"/>
-      <c r="E65" s="45"/>
-      <c r="G65" s="61" t="s">
-        <v>321</v>
+      <c r="C65" s="55" t="s">
+        <v>323</v>
+      </c>
+      <c r="E65" s="47"/>
+      <c r="G65" s="8" t="s">
+        <v>324</v>
       </c>
       <c r="H65" s="9"/>
       <c r="I65" s="9"/>
@@ -3139,16 +3184,17 @@
         <v>31</v>
       </c>
       <c r="B66" s="52" t="s">
-        <v>281</v>
-      </c>
-      <c r="C66" s="55" t="s">
-        <v>323</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="C66" s="52"/>
+      <c r="D66" s="44"/>
       <c r="E66" s="47"/>
       <c r="G66" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="H66" s="9"/>
+        <v>327</v>
+      </c>
+      <c r="H66" s="8" t="s">
+        <v>326</v>
+      </c>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
@@ -3160,15 +3206,15 @@
       <c r="B67" s="52" t="s">
         <v>326</v>
       </c>
-      <c r="C67" s="52"/>
+      <c r="C67" s="54" t="s">
+        <v>328</v>
+      </c>
       <c r="D67" s="44"/>
-      <c r="E67" s="47"/>
+      <c r="E67" s="45"/>
       <c r="G67" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="H67" s="8" t="s">
-        <v>326</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="H67" s="9"/>
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
@@ -3177,37 +3223,37 @@
       <c r="A68" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="52" t="s">
-        <v>326</v>
-      </c>
-      <c r="C68" s="54" t="s">
-        <v>328</v>
-      </c>
-      <c r="D68" s="44"/>
-      <c r="E68" s="45"/>
-      <c r="G68" s="8" t="s">
-        <v>330</v>
-      </c>
+      <c r="B68" s="59" t="s">
+        <v>331</v>
+      </c>
+      <c r="C68" s="59"/>
+      <c r="G68" s="9"/>
       <c r="H68" s="9"/>
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
     </row>
-    <row r="69" spans="1:11" ht="12.75">
+    <row r="69" spans="1:11" ht="14.25">
       <c r="A69" s="54" t="s">
         <v>31</v>
       </c>
       <c r="B69" s="59" t="s">
         <v>331</v>
       </c>
-      <c r="C69" s="59"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
+      <c r="C69" s="59" t="s">
+        <v>335</v>
+      </c>
+      <c r="G69" s="63" t="s">
+        <v>336</v>
+      </c>
+      <c r="H69" s="65" t="s">
+        <v>338</v>
+      </c>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
     </row>
-    <row r="70" spans="1:11" ht="14.25">
+    <row r="70" spans="1:11" ht="12.75">
       <c r="A70" s="54" t="s">
         <v>31</v>
       </c>
@@ -3215,14 +3261,12 @@
         <v>331</v>
       </c>
       <c r="C70" s="59" t="s">
-        <v>335</v>
-      </c>
-      <c r="G70" s="63" t="s">
-        <v>336</v>
-      </c>
-      <c r="H70" s="65" t="s">
-        <v>338</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="H70" s="9"/>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
@@ -3234,11 +3278,11 @@
       <c r="B71" s="59" t="s">
         <v>331</v>
       </c>
-      <c r="C71" s="59" t="s">
-        <v>339</v>
+      <c r="C71" s="58" t="s">
+        <v>341</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="H71" s="9"/>
       <c r="I71" s="9"/>
@@ -3250,13 +3294,11 @@
         <v>31</v>
       </c>
       <c r="B72" s="59" t="s">
-        <v>331</v>
-      </c>
-      <c r="C72" s="58" t="s">
-        <v>341</v>
-      </c>
-      <c r="G72" s="8" t="s">
-        <v>347</v>
+        <v>349</v>
+      </c>
+      <c r="C72" s="59"/>
+      <c r="G72" s="9" t="s">
+        <v>350</v>
       </c>
       <c r="H72" s="9"/>
       <c r="I72" s="9"/>
@@ -3268,11 +3310,11 @@
         <v>31</v>
       </c>
       <c r="B73" s="59" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="C73" s="59"/>
-      <c r="G73" s="9" t="s">
-        <v>350</v>
+      <c r="G73" s="8" t="s">
+        <v>354</v>
       </c>
       <c r="H73" s="9"/>
       <c r="I73" s="9"/>
@@ -3284,11 +3326,11 @@
         <v>31</v>
       </c>
       <c r="B74" s="59" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C74" s="59"/>
       <c r="G74" s="8" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
@@ -3300,11 +3342,11 @@
         <v>31</v>
       </c>
       <c r="B75" s="59" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="C75" s="59"/>
-      <c r="G75" s="8" t="s">
-        <v>358</v>
+      <c r="G75" s="9" t="s">
+        <v>360</v>
       </c>
       <c r="H75" s="9"/>
       <c r="I75" s="9"/>
@@ -3318,9 +3360,11 @@
       <c r="B76" s="59" t="s">
         <v>360</v>
       </c>
-      <c r="C76" s="59"/>
-      <c r="G76" s="9" t="s">
-        <v>360</v>
+      <c r="C76" s="58" t="s">
+        <v>362</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>364</v>
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="9"/>
@@ -3334,11 +3378,11 @@
       <c r="B77" s="59" t="s">
         <v>360</v>
       </c>
-      <c r="C77" s="58" t="s">
-        <v>362</v>
+      <c r="C77" s="67" t="s">
+        <v>365</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="H77" s="9"/>
       <c r="I77" s="9"/>
@@ -3346,18 +3390,6 @@
       <c r="K77" s="9"/>
     </row>
     <row r="78" spans="1:11" ht="12.75">
-      <c r="A78" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="B78" s="59" t="s">
-        <v>360</v>
-      </c>
-      <c r="C78" s="67" t="s">
-        <v>365</v>
-      </c>
-      <c r="G78" s="8" t="s">
-        <v>366</v>
-      </c>
       <c r="H78" s="9"/>
       <c r="I78" s="9"/>
       <c r="J78" s="9"/>
@@ -3448,6 +3480,7 @@
       <c r="K92" s="9"/>
     </row>
     <row r="93" spans="7:11" ht="12.75">
+      <c r="G93" s="9"/>
       <c r="H93" s="9"/>
       <c r="I93" s="9"/>
       <c r="J93" s="9"/>
@@ -9409,13 +9442,6 @@
       <c r="I944" s="9"/>
       <c r="J944" s="9"/>
       <c r="K944" s="9"/>
-    </row>
-    <row r="945" spans="7:11" ht="12.75">
-      <c r="G945" s="9"/>
-      <c r="H945" s="9"/>
-      <c r="I945" s="9"/>
-      <c r="J945" s="9"/>
-      <c r="K945" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9441,7 +9467,7 @@
     <col min="8" max="8" width="71.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
added longlists used in testing
</commit_message>
<xml_diff>
--- a/tool/sustainalize/Longlist V2.xlsx
+++ b/tool/sustainalize/Longlist V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hornr\source\repos\openmasses\tool\sustainalize\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{599A2454-975A-4541-BC9C-328996121CD9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BE7CA072-C148-481F-84F5-C988C8D9AD49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="419">
   <si>
     <t>Topic</t>
   </si>
@@ -1269,32 +1269,23 @@
     <t>Partnerships</t>
   </si>
   <si>
-    <t>thing1</t>
-  </si>
-  <si>
-    <t>thing2</t>
-  </si>
-  <si>
-    <t>thing3</t>
-  </si>
-  <si>
-    <t>thing4</t>
-  </si>
-  <si>
-    <t>thing5</t>
-  </si>
-  <si>
-    <t>thing6</t>
-  </si>
-  <si>
     <t>new  fancy knowledge creation</t>
+  </si>
+  <si>
+    <t>Fossil Fuels</t>
+  </si>
+  <si>
+    <t>Solar Energy</t>
+  </si>
+  <si>
+    <t>Nuclear Energy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1327,6 +1318,11 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Inconsolata"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1395,7 +1391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1481,6 +1477,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1800,9 +1801,9 @@
   </sheetPr>
   <dimension ref="A1:K944"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B45:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1877,7 +1878,7 @@
         <v>51</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
@@ -2441,8 +2442,8 @@
       <c r="B30" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="C30" s="43" t="s">
-        <v>415</v>
+      <c r="C30" s="71" t="s">
+        <v>180</v>
       </c>
       <c r="D30" s="32"/>
       <c r="E30" s="40"/>
@@ -2462,10 +2463,12 @@
       <c r="B31" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="C31" s="43" t="s">
-        <v>416</v>
-      </c>
-      <c r="D31" s="32"/>
+      <c r="C31" s="71" t="s">
+        <v>180</v>
+      </c>
+      <c r="D31" s="72" t="s">
+        <v>182</v>
+      </c>
       <c r="E31" s="33"/>
       <c r="F31" s="34"/>
       <c r="G31" s="35" t="s">
@@ -2483,11 +2486,15 @@
       <c r="B32" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="71" t="s">
+        <v>180</v>
+      </c>
+      <c r="D32" s="72" t="s">
+        <v>182</v>
+      </c>
+      <c r="E32" s="73" t="s">
         <v>417</v>
       </c>
-      <c r="D32" s="32"/>
-      <c r="E32" s="40"/>
       <c r="F32" s="34"/>
       <c r="G32" s="35" t="s">
         <v>187</v>
@@ -2501,14 +2508,18 @@
       <c r="A33" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="71" t="s">
         <v>177</v>
       </c>
-      <c r="C33" s="43" t="s">
+      <c r="C33" s="71" t="s">
+        <v>180</v>
+      </c>
+      <c r="D33" s="72" t="s">
+        <v>182</v>
+      </c>
+      <c r="E33" s="73" t="s">
         <v>418</v>
       </c>
-      <c r="D33" s="32"/>
-      <c r="E33" s="40"/>
       <c r="F33" s="34"/>
       <c r="G33" s="35" t="s">
         <v>189</v>
@@ -2525,10 +2536,12 @@
       <c r="B34" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="C34" s="43" t="s">
-        <v>419</v>
-      </c>
-      <c r="D34" s="32"/>
+      <c r="C34" s="71" t="s">
+        <v>180</v>
+      </c>
+      <c r="D34" s="72" t="s">
+        <v>416</v>
+      </c>
       <c r="E34" s="33"/>
       <c r="F34" s="34"/>
       <c r="G34" s="35" t="s">
@@ -2543,11 +2556,11 @@
       <c r="A35" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="71" t="s">
         <v>177</v>
       </c>
-      <c r="C35" s="43" t="s">
-        <v>420</v>
+      <c r="C35" s="71" t="s">
+        <v>192</v>
       </c>
       <c r="D35" s="32"/>
       <c r="E35" s="33"/>
@@ -9445,6 +9458,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>